<commit_message>
Added step definitions + feature files + updated pom
</commit_message>
<xml_diff>
--- a/dataForDDT.xlsx
+++ b/dataForDDT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="18960" windowHeight="4596"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,21 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>Sr. No</t>
+    <t>admin123</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Admin</t>
   </si>
   <si>
-    <t>Maverick</t>
+    <t>admin321</t>
   </si>
   <si>
-    <t>Goose</t>
-  </si>
-  <si>
-    <t>Ice</t>
+    <t>admin312</t>
   </si>
 </sst>
 </file>
@@ -362,24 +359,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="3" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -387,19 +387,11 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>